<commit_message>
mod3 cont to work
</commit_message>
<xml_diff>
--- a/Module 3 Equities and Currencies/Module 3 Exam/write-up/results.xlsx
+++ b/Module 3 Equities and Currencies/Module 3 Exam/write-up/results.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CQF\Module 3 Equities and Currencies\Module 3 Exam\write-up\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27798" windowHeight="14370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="13">
   <si>
     <t>Call</t>
   </si>
@@ -37,16 +42,49 @@
   </si>
   <si>
     <t>Floating</t>
+  </si>
+  <si>
+    <t>Theoretical Geo</t>
+  </si>
+  <si>
+    <t>% Diff</t>
+  </si>
+  <si>
+    <t>Theoretical Arith</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>\\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,23 +107,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -134,7 +181,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -167,9 +214,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -202,6 +266,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -378,15 +459,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F12"/>
+  <dimension ref="B2:AG16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AG8" sqref="R3:AG8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -398,8 +479,32 @@
         <v>4</v>
       </c>
       <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -415,8 +520,84 @@
       <c r="F3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>1000</v>
+      </c>
+      <c r="J3">
+        <v>5.6990999999999996</v>
+      </c>
+      <c r="K3">
+        <v>5.7827999999999999</v>
+      </c>
+      <c r="L3" s="2">
+        <f>J3/K3-1</f>
+        <v>-1.447395725254208E-2</v>
+      </c>
+      <c r="M3">
+        <v>5.4916</v>
+      </c>
+      <c r="N3">
+        <v>5.5468000000000002</v>
+      </c>
+      <c r="O3" s="2">
+        <f>M3/N3-1</f>
+        <v>-9.9516838537535568E-3</v>
+      </c>
+      <c r="R3" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" t="s">
+        <v>11</v>
+      </c>
+      <c r="T3">
+        <v>1000</v>
+      </c>
+      <c r="U3" t="s">
+        <v>11</v>
+      </c>
+      <c r="V3">
+        <v>5.6990999999999996</v>
+      </c>
+      <c r="W3" t="s">
+        <v>11</v>
+      </c>
+      <c r="X3">
+        <v>5.7827999999999999</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z3" s="2">
+        <f>V3/X3-1</f>
+        <v>-1.447395725254208E-2</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB3">
+        <v>5.4916</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD3">
+        <v>5.5468000000000002</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF3" s="2">
+        <f>AB3/AD3-1</f>
+        <v>-9.9516838537535568E-3</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B4">
         <v>1000</v>
       </c>
@@ -432,8 +613,82 @@
       <c r="F4">
         <v>3.4247999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H4" s="1"/>
+      <c r="I4">
+        <v>10000</v>
+      </c>
+      <c r="J4">
+        <v>5.7328000000000001</v>
+      </c>
+      <c r="K4">
+        <v>5.7827999999999999</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" ref="L4:L5" si="0">J4/K4-1</f>
+        <v>-8.6463304973368738E-3</v>
+      </c>
+      <c r="M4">
+        <v>5.5180999999999996</v>
+      </c>
+      <c r="N4">
+        <v>5.5468000000000002</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" ref="O4:O5" si="1">M4/N4-1</f>
+        <v>-5.1741544674408502E-3</v>
+      </c>
+      <c r="R4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S4" t="s">
+        <v>11</v>
+      </c>
+      <c r="T4">
+        <v>10000</v>
+      </c>
+      <c r="U4" t="s">
+        <v>11</v>
+      </c>
+      <c r="V4">
+        <v>5.7328000000000001</v>
+      </c>
+      <c r="W4" t="s">
+        <v>11</v>
+      </c>
+      <c r="X4">
+        <v>5.7827999999999999</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z4" s="2">
+        <f t="shared" ref="Z4:Z5" si="2">V4/X4-1</f>
+        <v>-8.6463304973368738E-3</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB4">
+        <v>5.5180999999999996</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD4">
+        <v>5.5468000000000002</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF4" s="2">
+        <f t="shared" ref="AF4:AF5" si="3">AB4/AD4-1</f>
+        <v>-5.1741544674408502E-3</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B5">
         <v>10000</v>
       </c>
@@ -449,8 +704,82 @@
       <c r="F5">
         <v>3.4415</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H5" s="1"/>
+      <c r="I5">
+        <v>100000</v>
+      </c>
+      <c r="J5">
+        <v>5.7423999999999999</v>
+      </c>
+      <c r="K5">
+        <v>5.7827999999999999</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" si="0"/>
+        <v>-6.9862350418482544E-3</v>
+      </c>
+      <c r="M5">
+        <v>5.5262000000000002</v>
+      </c>
+      <c r="N5">
+        <v>5.5468000000000002</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.7138530323790331E-3</v>
+      </c>
+      <c r="R5" t="s">
+        <v>0</v>
+      </c>
+      <c r="S5" t="s">
+        <v>11</v>
+      </c>
+      <c r="T5">
+        <v>100000</v>
+      </c>
+      <c r="U5" t="s">
+        <v>11</v>
+      </c>
+      <c r="V5">
+        <v>5.7423999999999999</v>
+      </c>
+      <c r="W5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X5">
+        <v>5.7827999999999999</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z5" s="2">
+        <f t="shared" si="2"/>
+        <v>-6.9862350418482544E-3</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB5">
+        <v>5.5262000000000002</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD5">
+        <v>5.5468000000000002</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF5" s="2">
+        <f t="shared" si="3"/>
+        <v>-3.7138530323790331E-3</v>
+      </c>
+      <c r="AG5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B6">
         <v>100000</v>
       </c>
@@ -466,8 +795,160 @@
       <c r="F6">
         <v>3.4464999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>1000</v>
+      </c>
+      <c r="J6">
+        <v>3.3107000000000002</v>
+      </c>
+      <c r="K6">
+        <v>3.3645999999999998</v>
+      </c>
+      <c r="L6" s="2">
+        <f>J6/K6-1</f>
+        <v>-1.6019734886762005E-2</v>
+      </c>
+      <c r="M6">
+        <v>3.4247999999999998</v>
+      </c>
+      <c r="N6">
+        <v>3.4632999999999998</v>
+      </c>
+      <c r="O6" s="2">
+        <f>M6/N6-1</f>
+        <v>-1.1116565125747102E-2</v>
+      </c>
+      <c r="R6" t="s">
+        <v>4</v>
+      </c>
+      <c r="S6" t="s">
+        <v>11</v>
+      </c>
+      <c r="T6">
+        <v>1000</v>
+      </c>
+      <c r="U6" t="s">
+        <v>11</v>
+      </c>
+      <c r="V6">
+        <v>3.3107000000000002</v>
+      </c>
+      <c r="W6" t="s">
+        <v>11</v>
+      </c>
+      <c r="X6">
+        <v>3.3645999999999998</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z6" s="2">
+        <f>V6/X6-1</f>
+        <v>-1.6019734886762005E-2</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB6">
+        <v>3.4247999999999998</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD6">
+        <v>3.4632999999999998</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF6" s="2">
+        <f>AB6/AD6-1</f>
+        <v>-1.1116565125747102E-2</v>
+      </c>
+      <c r="AG6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="H7" s="1"/>
+      <c r="I7">
+        <v>10000</v>
+      </c>
+      <c r="J7">
+        <v>3.3237999999999999</v>
+      </c>
+      <c r="K7">
+        <v>3.3645999999999998</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" ref="L7:L8" si="4">J7/K7-1</f>
+        <v>-1.2126255721333856E-2</v>
+      </c>
+      <c r="M7">
+        <v>3.4415</v>
+      </c>
+      <c r="N7">
+        <v>3.4632999999999998</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" ref="O7:O8" si="5">M7/N7-1</f>
+        <v>-6.2945745387347207E-3</v>
+      </c>
+      <c r="R7" t="s">
+        <v>4</v>
+      </c>
+      <c r="S7" t="s">
+        <v>11</v>
+      </c>
+      <c r="T7">
+        <v>10000</v>
+      </c>
+      <c r="U7" t="s">
+        <v>11</v>
+      </c>
+      <c r="V7">
+        <v>3.3237999999999999</v>
+      </c>
+      <c r="W7" t="s">
+        <v>11</v>
+      </c>
+      <c r="X7">
+        <v>3.3645999999999998</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z7" s="2">
+        <f t="shared" ref="Z7:Z8" si="6">V7/X7-1</f>
+        <v>-1.2126255721333856E-2</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB7">
+        <v>3.4415</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD7">
+        <v>3.4632999999999998</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF7" s="2">
+        <f t="shared" ref="AF7:AF8" si="7">AB7/AD7-1</f>
+        <v>-6.2945745387347207E-3</v>
+      </c>
+      <c r="AG7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -479,8 +960,82 @@
         <v>4</v>
       </c>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H8" s="1"/>
+      <c r="I8">
+        <v>100000</v>
+      </c>
+      <c r="J8">
+        <v>3.3285</v>
+      </c>
+      <c r="K8">
+        <v>3.3645999999999998</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="4"/>
+        <v>-1.0729358616180185E-2</v>
+      </c>
+      <c r="M8">
+        <v>3.4464999999999999</v>
+      </c>
+      <c r="N8">
+        <v>3.4632999999999998</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="5"/>
+        <v>-4.8508647821441375E-3</v>
+      </c>
+      <c r="R8" t="s">
+        <v>4</v>
+      </c>
+      <c r="S8" t="s">
+        <v>11</v>
+      </c>
+      <c r="T8">
+        <v>100000</v>
+      </c>
+      <c r="U8" t="s">
+        <v>11</v>
+      </c>
+      <c r="V8">
+        <v>3.3285</v>
+      </c>
+      <c r="W8" t="s">
+        <v>11</v>
+      </c>
+      <c r="X8">
+        <v>3.3645999999999998</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z8" s="2">
+        <f t="shared" si="6"/>
+        <v>-1.0729358616180185E-2</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB8">
+        <v>3.4464999999999999</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD8">
+        <v>3.4632999999999998</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF8" s="2">
+        <f t="shared" si="7"/>
+        <v>-4.8508647821441375E-3</v>
+      </c>
+      <c r="AG8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -497,7 +1052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B10">
         <v>1000</v>
       </c>
@@ -514,7 +1069,7 @@
         <v>3.2349000000000001</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B11">
         <v>10000</v>
       </c>
@@ -530,8 +1085,10 @@
       <c r="F11">
         <v>3.2528000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="L11" s="2"/>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B12">
         <v>100000</v>
       </c>
@@ -547,16 +1104,40 @@
       <c r="F12">
         <v>3.2692000000000001</v>
       </c>
+      <c r="L12" s="2"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="L13" s="2"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="L14" s="2"/>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="L15" s="2"/>
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="L16" s="2"/>
+      <c r="O16" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="H6:H8"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="AG3" r:id="rId1"/>
+    <hyperlink ref="AG4:AG8" r:id="rId2" display="\\"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -566,7 +1147,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -578,7 +1159,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>